<commit_message>
Changes in Defect report, Defect creation in TFS and Defect report exception handlng change
</commit_message>
<xml_diff>
--- a/iTF/keywords/HomaUserManagement.xlsx
+++ b/iTF/keywords/HomaUserManagement.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70648" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76526" uniqueCount="88">
   <si>
     <t>Test Scenario</t>
   </si>
@@ -782,7 +782,7 @@
         <v>27</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>31</v>
@@ -824,7 +824,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>31</v>
@@ -856,7 +856,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>31</v>
@@ -888,7 +888,7 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>31</v>

</xml_diff>